<commit_message>
Chicaog Violent crime is the current R-script that I am working on. This is where all the analyzation will take place. The animated time series is on it, ignore the codes in the very end. CrimeProject script is simply the script where i analyzed and subsetted the data. this script no longer needs to be adjusted. the Data sources is excel sheet to be used to keep track of our data sources.
</commit_message>
<xml_diff>
--- a/Data Sources.xlsx
+++ b/Data Sources.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="460" windowWidth="21820" windowHeight="14640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3780" yWindow="460" windowWidth="21820" windowHeight="14640" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resources of Links" sheetId="1" r:id="rId1"/>
-    <sheet name="Description of Crimes" sheetId="2" r:id="rId2"/>
+    <sheet name="Description of Crimes (Chicago)" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Exploration" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
   <si>
     <t>Crime</t>
   </si>
@@ -226,6 +227,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Unlawful, nonviolent acts by a family member (or legal guardian) that threaten the physical, mental, or economic well-being or morals of another family member and that are not classifiable as other offenses, such as Assault, Incest, Statutory Rape, etc.</t>
+  </si>
+  <si>
+    <t>6340790 x 22</t>
+  </si>
+  <si>
+    <t>Total Dimension (2010 - Current)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Dimensions (2001 - Current): </t>
+  </si>
+  <si>
+    <t>2264846 x 24</t>
   </si>
 </sst>
 </file>
@@ -695,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,4 +961,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>